<commit_message>
opened these files, didn't make any changes
</commit_message>
<xml_diff>
--- a/analysis/data/raw_data/2016_Final_ModelingData_Steelhead.xlsx
+++ b/analysis/data/raw_data/2016_Final_ModelingData_Steelhead.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28315"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevin/Dropbox/ISEMP/Analysis_Projects/Wenatchee_ReddCounts/Steelhead_2016/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stateofwa-my.sharepoint.com/personal/kevin_see_dfw_wa_gov/Documents/Documents/Git/MyProjects/UCSthdReddObsErr/analysis/data/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_7F4A91476675EE85A5752249DFB574F3EBFB9C82" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{81B60EFA-35B1-45F8-9740-676BA0D19750}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="460" windowWidth="13400" windowHeight="7500"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Survey Data-Working" sheetId="4" r:id="rId1"/>
@@ -21,10 +22,21 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Redd Life'!$A$2:$H$112</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Survey Data-Working'!$A$1:$AI$160</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -34,12 +46,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>CD-WDFW</author>
   </authors>
   <commentList>
-    <comment ref="F23" authorId="0">
+    <comment ref="F23" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -805,7 +817,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
     <numFmt numFmtId="165" formatCode="h:mm;@"/>
@@ -1563,13 +1575,16 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal_Sheet1" xfId="1"/>
+    <cellStyle name="Normal_Sheet1" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1861,7 +1876,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD160"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -1870,34 +1885,34 @@
       <selection pane="bottomLeft" activeCell="R98" sqref="R98"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="11.5" style="15"/>
-    <col min="3" max="3" width="7.5" style="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="11.5" style="15"/>
-    <col min="6" max="6" width="11.5" style="17"/>
-    <col min="7" max="10" width="11.5" style="23"/>
-    <col min="11" max="11" width="11.5" style="27"/>
-    <col min="12" max="12" width="4.6640625" style="17" customWidth="1"/>
-    <col min="13" max="13" width="4.5" style="17" customWidth="1"/>
-    <col min="14" max="14" width="7.5" style="20" customWidth="1"/>
-    <col min="15" max="15" width="11.5" style="20"/>
-    <col min="16" max="16" width="11.5" style="23"/>
-    <col min="17" max="17" width="4.83203125" style="17" customWidth="1"/>
-    <col min="18" max="18" width="4.6640625" style="17" customWidth="1"/>
-    <col min="19" max="19" width="7.5" style="23" customWidth="1"/>
-    <col min="20" max="20" width="8.5" style="23" customWidth="1"/>
-    <col min="21" max="21" width="11.5" style="20"/>
-    <col min="22" max="23" width="11.5" style="15"/>
-    <col min="24" max="24" width="14.1640625" style="21" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.5" style="15"/>
-    <col min="26" max="26" width="11.5" style="20"/>
-    <col min="27" max="27" width="11.5" style="15"/>
-    <col min="28" max="28" width="26.6640625" style="15" bestFit="1" customWidth="1"/>
-    <col min="29" max="16384" width="11.5" style="15"/>
+    <col min="1" max="2" width="11.453125" style="15"/>
+    <col min="3" max="3" width="7.453125" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11.453125" style="15"/>
+    <col min="6" max="6" width="11.453125" style="17"/>
+    <col min="7" max="10" width="11.453125" style="23"/>
+    <col min="11" max="11" width="11.453125" style="27"/>
+    <col min="12" max="12" width="4.6328125" style="17" customWidth="1"/>
+    <col min="13" max="13" width="4.453125" style="17" customWidth="1"/>
+    <col min="14" max="14" width="7.453125" style="20" customWidth="1"/>
+    <col min="15" max="15" width="11.453125" style="20"/>
+    <col min="16" max="16" width="11.453125" style="23"/>
+    <col min="17" max="17" width="4.81640625" style="17" customWidth="1"/>
+    <col min="18" max="18" width="4.6328125" style="17" customWidth="1"/>
+    <col min="19" max="19" width="7.453125" style="23" customWidth="1"/>
+    <col min="20" max="20" width="8.453125" style="23" customWidth="1"/>
+    <col min="21" max="21" width="11.453125" style="20"/>
+    <col min="22" max="23" width="11.453125" style="15"/>
+    <col min="24" max="24" width="14.1796875" style="21" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.453125" style="15"/>
+    <col min="26" max="26" width="11.453125" style="20"/>
+    <col min="27" max="27" width="11.453125" style="15"/>
+    <col min="28" max="28" width="26.6328125" style="15" bestFit="1" customWidth="1"/>
+    <col min="29" max="16384" width="11.453125" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" ht="48.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -1983,7 +1998,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A2" s="109" t="s">
         <v>18</v>
       </c>
@@ -2073,7 +2088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A3" s="109" t="s">
         <v>19</v>
       </c>
@@ -2141,7 +2156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A4" s="109" t="s">
         <v>18</v>
       </c>
@@ -2231,7 +2246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A5" s="109" t="s">
         <v>21</v>
       </c>
@@ -2299,7 +2314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A6" s="109" t="s">
         <v>18</v>
       </c>
@@ -2389,7 +2404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A7" s="109" t="s">
         <v>18</v>
       </c>
@@ -2479,7 +2494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A8" s="109" t="s">
         <v>18</v>
       </c>
@@ -2569,7 +2584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A9" s="109" t="s">
         <v>18</v>
       </c>
@@ -2659,7 +2674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A10" s="109" t="s">
         <v>20</v>
       </c>
@@ -2727,7 +2742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A11" s="109" t="s">
         <v>19</v>
       </c>
@@ -2795,7 +2810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A12" s="109" t="s">
         <v>18</v>
       </c>
@@ -2885,7 +2900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A13" s="109" t="s">
         <v>21</v>
       </c>
@@ -2953,7 +2968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="109" t="s">
         <v>18</v>
       </c>
@@ -3043,7 +3058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="109" t="s">
         <v>18</v>
       </c>
@@ -3133,7 +3148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A16" s="109" t="s">
         <v>18</v>
       </c>
@@ -3223,7 +3238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A17" s="109" t="s">
         <v>18</v>
       </c>
@@ -3313,7 +3328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A18" s="109" t="s">
         <v>20</v>
       </c>
@@ -3381,7 +3396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="109" t="s">
         <v>19</v>
       </c>
@@ -3449,7 +3464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="109" t="s">
         <v>18</v>
       </c>
@@ -3539,7 +3554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A21" s="109" t="s">
         <v>21</v>
       </c>
@@ -3607,7 +3622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A22" s="109" t="s">
         <v>18</v>
       </c>
@@ -3697,7 +3712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A23" s="109" t="s">
         <v>18</v>
       </c>
@@ -3787,7 +3802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A24" s="109" t="s">
         <v>18</v>
       </c>
@@ -3877,7 +3892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A25" s="109" t="s">
         <v>18</v>
       </c>
@@ -3967,7 +3982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A26" s="109" t="s">
         <v>20</v>
       </c>
@@ -4038,7 +4053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:28" s="26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:28" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="109" t="s">
         <v>19</v>
       </c>
@@ -4109,7 +4124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A28" s="109" t="s">
         <v>18</v>
       </c>
@@ -4199,7 +4214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A29" s="109" t="s">
         <v>21</v>
       </c>
@@ -4270,7 +4285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A30" s="109" t="s">
         <v>18</v>
       </c>
@@ -4360,7 +4375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A31" s="109" t="s">
         <v>18</v>
       </c>
@@ -4450,7 +4465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A32" s="109" t="s">
         <v>18</v>
       </c>
@@ -4540,7 +4555,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A33" s="109" t="s">
         <v>18</v>
       </c>
@@ -4630,7 +4645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A34" s="109" t="s">
         <v>18</v>
       </c>
@@ -4720,7 +4735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A35" s="109" t="s">
         <v>21</v>
       </c>
@@ -4791,7 +4806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A36" s="109" t="s">
         <v>19</v>
       </c>
@@ -4859,7 +4874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A37" s="109" t="s">
         <v>18</v>
       </c>
@@ -4949,7 +4964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:30" s="26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:30" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A38" s="109" t="s">
         <v>18</v>
       </c>
@@ -5039,7 +5054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A39" s="109" t="s">
         <v>18</v>
       </c>
@@ -5129,7 +5144,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="40" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A40" s="109" t="s">
         <v>18</v>
       </c>
@@ -5219,7 +5234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A41" s="109" t="s">
         <v>18</v>
       </c>
@@ -5309,7 +5324,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A42" s="109" t="s">
         <v>18</v>
       </c>
@@ -5399,7 +5414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A43" s="109" t="s">
         <v>18</v>
       </c>
@@ -5489,7 +5504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A44" s="109" t="s">
         <v>18</v>
       </c>
@@ -5580,7 +5595,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="45" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A45" s="109" t="s">
         <v>18</v>
       </c>
@@ -5670,7 +5685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A46" s="109" t="s">
         <v>18</v>
       </c>
@@ -5760,7 +5775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A47" s="109" t="s">
         <v>18</v>
       </c>
@@ -5853,7 +5868,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="48" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A48" s="109" t="s">
         <v>18</v>
       </c>
@@ -5943,7 +5958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A49" s="109" t="s">
         <v>18</v>
       </c>
@@ -6033,7 +6048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:28" s="16" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:28" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A50" s="109" t="s">
         <v>18</v>
       </c>
@@ -6123,7 +6138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="109" t="s">
         <v>18</v>
       </c>
@@ -6213,7 +6228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="109" t="s">
         <v>18</v>
       </c>
@@ -6303,7 +6318,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A53" s="109" t="s">
         <v>20</v>
       </c>
@@ -6374,7 +6389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A54" s="109" t="s">
         <v>19</v>
       </c>
@@ -6442,7 +6457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A55" s="109" t="s">
         <v>18</v>
       </c>
@@ -6532,7 +6547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A56" s="109" t="s">
         <v>18</v>
       </c>
@@ -6622,7 +6637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A57" s="109" t="s">
         <v>18</v>
       </c>
@@ -6712,7 +6727,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A58" s="109" t="s">
         <v>21</v>
       </c>
@@ -6783,7 +6798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A59" s="109" t="s">
         <v>18</v>
       </c>
@@ -6873,7 +6888,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A60" s="109" t="s">
         <v>19</v>
       </c>
@@ -6941,7 +6956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A61" s="109" t="s">
         <v>18</v>
       </c>
@@ -7031,7 +7046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A62" s="109" t="s">
         <v>21</v>
       </c>
@@ -7102,7 +7117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A63" s="109" t="s">
         <v>18</v>
       </c>
@@ -7192,7 +7207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A64" s="109" t="s">
         <v>18</v>
       </c>
@@ -7282,7 +7297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A65" s="109" t="s">
         <v>18</v>
       </c>
@@ -7372,7 +7387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A66" s="109" t="s">
         <v>18</v>
       </c>
@@ -7462,7 +7477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A67" s="109" t="s">
         <v>18</v>
       </c>
@@ -7552,7 +7567,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="68" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A68" s="109" t="s">
         <v>18</v>
       </c>
@@ -7642,7 +7657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A69" s="109" t="s">
         <v>18</v>
       </c>
@@ -7732,7 +7747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A70" s="109" t="s">
         <v>18</v>
       </c>
@@ -7822,7 +7837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:28" s="109" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:28" s="109" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A71" s="109" t="s">
         <v>19</v>
       </c>
@@ -7893,7 +7908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:28" s="109" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:28" s="109" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A72" s="109" t="s">
         <v>21</v>
       </c>
@@ -7967,7 +7982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:28" s="109" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:28" s="109" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A73" s="109" t="s">
         <v>18</v>
       </c>
@@ -8057,7 +8072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A74" s="109" t="s">
         <v>18</v>
       </c>
@@ -8147,7 +8162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A75" s="109" t="s">
         <v>18</v>
       </c>
@@ -8237,7 +8252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A76" s="109" t="s">
         <v>18</v>
       </c>
@@ -8327,7 +8342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A77" s="109" t="s">
         <v>18</v>
       </c>
@@ -8417,7 +8432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A78" s="109" t="s">
         <v>18</v>
       </c>
@@ -8507,7 +8522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A79" s="109" t="s">
         <v>20</v>
       </c>
@@ -8578,7 +8593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A80" s="109" t="s">
         <v>19</v>
       </c>
@@ -8646,7 +8661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A81" s="109" t="s">
         <v>18</v>
       </c>
@@ -8736,7 +8751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A82" s="109" t="s">
         <v>21</v>
       </c>
@@ -8807,7 +8822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A83" s="109" t="s">
         <v>18</v>
       </c>
@@ -8897,7 +8912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A84" s="109" t="s">
         <v>18</v>
       </c>
@@ -8987,7 +9002,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A85" s="109" t="s">
         <v>19</v>
       </c>
@@ -9055,7 +9070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A86" s="109" t="s">
         <v>21</v>
       </c>
@@ -9126,7 +9141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A87" s="109" t="s">
         <v>18</v>
       </c>
@@ -9216,7 +9231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A88" s="109" t="s">
         <v>20</v>
       </c>
@@ -9287,7 +9302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A89" s="109" t="s">
         <v>18</v>
       </c>
@@ -9377,7 +9392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A90" s="109" t="s">
         <v>18</v>
       </c>
@@ -9467,7 +9482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A91" s="109" t="s">
         <v>18</v>
       </c>
@@ -9557,286 +9572,286 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:28" x14ac:dyDescent="0.35">
       <c r="E92" s="24"/>
       <c r="F92" s="39"/>
     </row>
-    <row r="93" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:28" x14ac:dyDescent="0.35">
       <c r="E93" s="24"/>
       <c r="F93" s="39"/>
     </row>
-    <row r="94" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:28" x14ac:dyDescent="0.35">
       <c r="E94" s="24"/>
       <c r="F94" s="39"/>
       <c r="K94" s="25"/>
     </row>
-    <row r="95" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:28" x14ac:dyDescent="0.35">
       <c r="E95" s="24"/>
       <c r="F95" s="39"/>
     </row>
-    <row r="96" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:28" x14ac:dyDescent="0.35">
       <c r="E96" s="24"/>
       <c r="F96" s="39"/>
     </row>
-    <row r="97" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="97" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E97" s="24"/>
       <c r="F97" s="39"/>
     </row>
-    <row r="98" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="98" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E98" s="24"/>
       <c r="F98" s="39"/>
     </row>
-    <row r="99" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="99" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E99" s="24"/>
       <c r="F99" s="39"/>
     </row>
-    <row r="100" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="100" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E100" s="24"/>
       <c r="F100" s="39"/>
     </row>
-    <row r="101" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="101" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E101" s="24"/>
       <c r="F101" s="39"/>
     </row>
-    <row r="102" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="102" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E102" s="24"/>
       <c r="F102" s="39"/>
     </row>
-    <row r="103" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="103" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E103" s="24"/>
       <c r="F103" s="39"/>
     </row>
-    <row r="104" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="104" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E104" s="24"/>
       <c r="F104" s="39"/>
     </row>
-    <row r="105" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="105" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E105" s="24"/>
       <c r="F105" s="39"/>
     </row>
-    <row r="106" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="106" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E106" s="24"/>
       <c r="F106" s="39"/>
     </row>
-    <row r="107" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="107" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E107" s="24"/>
       <c r="F107" s="39"/>
     </row>
-    <row r="108" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="108" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E108" s="24"/>
       <c r="F108" s="39"/>
     </row>
-    <row r="109" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="109" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E109" s="24"/>
       <c r="F109" s="39"/>
     </row>
-    <row r="110" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="110" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E110" s="24"/>
       <c r="F110" s="39"/>
     </row>
-    <row r="111" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="111" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E111" s="24"/>
       <c r="F111" s="39"/>
     </row>
-    <row r="112" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="112" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E112" s="24"/>
       <c r="F112" s="39"/>
     </row>
-    <row r="113" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="113" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E113" s="24"/>
       <c r="F113" s="39"/>
     </row>
-    <row r="114" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="114" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E114" s="24"/>
       <c r="F114" s="39"/>
     </row>
-    <row r="115" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="115" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E115" s="24"/>
       <c r="F115" s="39"/>
     </row>
-    <row r="116" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="116" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E116" s="24"/>
       <c r="F116" s="39"/>
     </row>
-    <row r="117" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="117" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E117" s="24"/>
       <c r="F117" s="39"/>
     </row>
-    <row r="118" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="118" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E118" s="24"/>
       <c r="F118" s="39"/>
     </row>
-    <row r="119" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="119" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E119" s="24"/>
       <c r="F119" s="39"/>
     </row>
-    <row r="120" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="120" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E120" s="24"/>
       <c r="F120" s="39"/>
     </row>
-    <row r="121" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="121" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E121" s="24"/>
       <c r="F121" s="39"/>
     </row>
-    <row r="122" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="122" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E122" s="24"/>
       <c r="F122" s="39"/>
     </row>
-    <row r="123" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="123" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E123" s="24"/>
       <c r="F123" s="39"/>
     </row>
-    <row r="124" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="124" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E124" s="24"/>
       <c r="F124" s="39"/>
     </row>
-    <row r="125" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="125" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E125" s="24"/>
       <c r="F125" s="39"/>
     </row>
-    <row r="126" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="126" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E126" s="24"/>
       <c r="F126" s="39"/>
     </row>
-    <row r="127" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="127" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E127" s="24"/>
       <c r="F127" s="39"/>
     </row>
-    <row r="128" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="128" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E128" s="24"/>
       <c r="F128" s="39"/>
     </row>
-    <row r="129" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="129" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E129" s="24"/>
       <c r="F129" s="39"/>
     </row>
-    <row r="130" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="130" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E130" s="24"/>
       <c r="F130" s="39"/>
     </row>
-    <row r="131" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="131" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E131" s="24"/>
       <c r="F131" s="39"/>
     </row>
-    <row r="132" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="132" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E132" s="24"/>
       <c r="F132" s="39"/>
     </row>
-    <row r="133" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="133" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E133" s="24"/>
       <c r="F133" s="39"/>
     </row>
-    <row r="134" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="134" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E134" s="24"/>
       <c r="F134" s="39"/>
     </row>
-    <row r="135" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="135" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E135" s="24"/>
       <c r="F135" s="39"/>
     </row>
-    <row r="136" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="136" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E136" s="24"/>
       <c r="F136" s="39"/>
     </row>
-    <row r="137" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="137" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E137" s="24"/>
       <c r="F137" s="39"/>
     </row>
-    <row r="138" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="138" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E138" s="24"/>
       <c r="F138" s="39"/>
     </row>
-    <row r="139" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="139" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E139" s="24"/>
       <c r="F139" s="39"/>
     </row>
-    <row r="140" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="140" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E140" s="24"/>
       <c r="F140" s="39"/>
     </row>
-    <row r="141" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="141" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E141" s="24"/>
       <c r="F141" s="39"/>
     </row>
-    <row r="142" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="142" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E142" s="24"/>
       <c r="F142" s="39"/>
     </row>
-    <row r="143" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="143" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E143" s="24"/>
       <c r="F143" s="39"/>
     </row>
-    <row r="144" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="144" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E144" s="24"/>
       <c r="F144" s="39"/>
     </row>
-    <row r="145" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="145" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E145" s="24"/>
       <c r="F145" s="39"/>
     </row>
-    <row r="146" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="146" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E146" s="24"/>
       <c r="F146" s="39"/>
     </row>
-    <row r="147" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="147" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E147" s="24"/>
       <c r="F147" s="39"/>
     </row>
-    <row r="148" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="148" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E148" s="24"/>
       <c r="F148" s="39"/>
     </row>
-    <row r="149" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="149" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E149" s="24"/>
       <c r="F149" s="39"/>
     </row>
-    <row r="150" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="150" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E150" s="24"/>
       <c r="F150" s="39"/>
     </row>
-    <row r="151" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="151" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E151" s="24"/>
       <c r="F151" s="39"/>
     </row>
-    <row r="152" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="152" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E152" s="24"/>
       <c r="F152" s="39"/>
     </row>
-    <row r="153" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="153" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E153" s="24"/>
       <c r="F153" s="39"/>
     </row>
-    <row r="154" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="154" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E154" s="24"/>
       <c r="F154" s="39"/>
     </row>
-    <row r="155" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="155" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E155" s="24"/>
       <c r="F155" s="39"/>
     </row>
-    <row r="156" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="156" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E156" s="24"/>
       <c r="F156" s="39"/>
     </row>
-    <row r="157" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="157" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E157" s="24"/>
       <c r="F157" s="39"/>
     </row>
-    <row r="158" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="158" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E158" s="24"/>
       <c r="F158" s="39"/>
     </row>
-    <row r="159" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="159" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E159" s="24"/>
       <c r="F159" s="39"/>
     </row>
-    <row r="160" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="160" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E160" s="24"/>
       <c r="F160" s="39"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AI160"/>
-  <sortState ref="A2:R213">
+  <autoFilter ref="A1:AI160" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R213">
     <sortCondition ref="B2:B213"/>
   </sortState>
   <dataConsolidate>
@@ -9850,39 +9865,39 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AB195"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="AA29" sqref="AA29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" customWidth="1"/>
-    <col min="5" max="5" width="12.5" style="42" customWidth="1"/>
+    <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6328125" customWidth="1"/>
+    <col min="5" max="5" width="12.453125" style="42" customWidth="1"/>
     <col min="6" max="6" width="11" style="42" customWidth="1"/>
     <col min="7" max="7" width="13" style="42" customWidth="1"/>
-    <col min="11" max="11" width="9.83203125" customWidth="1"/>
-    <col min="12" max="12" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.6640625" style="16" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.5" style="17" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.1640625" style="17" customWidth="1"/>
-    <col min="16" max="16" width="10.83203125" style="17" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.5" style="17" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.5" style="17" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.5" style="17" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.83203125" style="17" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.5" style="17" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.5" style="16" customWidth="1"/>
-    <col min="23" max="23" width="12.83203125" style="16" customWidth="1"/>
-    <col min="24" max="24" width="14.5" style="16" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9.6640625" style="16" bestFit="1" customWidth="1"/>
-    <col min="26" max="28" width="8.83203125" style="16"/>
+    <col min="11" max="11" width="9.81640625" customWidth="1"/>
+    <col min="12" max="12" width="6.6328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.6328125" style="16" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.453125" style="17" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.1796875" style="17" customWidth="1"/>
+    <col min="16" max="16" width="10.81640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.453125" style="17" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.453125" style="17" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.453125" style="17" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.81640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.453125" style="17" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.453125" style="16" customWidth="1"/>
+    <col min="23" max="23" width="12.81640625" style="16" customWidth="1"/>
+    <col min="24" max="24" width="14.453125" style="16" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.6328125" style="16" bestFit="1" customWidth="1"/>
+    <col min="26" max="28" width="8.81640625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E1" s="42"/>
       <c r="F1" s="42"/>
       <c r="G1" s="42"/>
@@ -9909,7 +9924,7 @@
       <c r="AA1" s="40"/>
       <c r="AB1" s="40"/>
     </row>
-    <row r="2" spans="1:28" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:28" ht="48" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>32</v>
       </c>
@@ -9978,7 +9993,7 @@
       <c r="AA2" s="45"/>
       <c r="AB2" s="44"/>
     </row>
-    <row r="3" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="135">
         <v>2016</v>
       </c>
@@ -10054,7 +10069,7 @@
       <c r="AA3" s="18"/>
       <c r="AB3" s="9"/>
     </row>
-    <row r="4" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="135">
         <v>2016</v>
       </c>
@@ -10127,7 +10142,7 @@
       <c r="AA4" s="9"/>
       <c r="AB4" s="9"/>
     </row>
-    <row r="5" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="135">
         <v>2016</v>
       </c>
@@ -10197,7 +10212,7 @@
       </c>
       <c r="Y5" s="22"/>
     </row>
-    <row r="6" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="135">
         <v>2016</v>
       </c>
@@ -10267,7 +10282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:28" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:28" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="135">
         <v>2016</v>
       </c>
@@ -10341,7 +10356,7 @@
       <c r="AA7" s="16"/>
       <c r="AB7" s="16"/>
     </row>
-    <row r="8" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="135">
         <v>2016</v>
       </c>
@@ -10411,7 +10426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="135">
         <v>2016</v>
       </c>
@@ -10481,7 +10496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="135">
         <v>2016</v>
       </c>
@@ -10551,7 +10566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="135">
         <v>2016</v>
       </c>
@@ -10621,7 +10636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="135">
         <v>2016</v>
       </c>
@@ -10695,7 +10710,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="13" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="135">
         <v>2016</v>
       </c>
@@ -10761,7 +10776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="135">
         <v>2016</v>
       </c>
@@ -10836,7 +10851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="135">
         <v>2016</v>
       </c>
@@ -10908,7 +10923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="135">
         <v>2016</v>
       </c>
@@ -10980,7 +10995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="135">
         <v>2016</v>
       </c>
@@ -11052,7 +11067,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="135">
         <v>2016</v>
       </c>
@@ -11117,7 +11132,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="135">
         <v>2016</v>
       </c>
@@ -11189,7 +11204,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="135">
         <v>2016</v>
       </c>
@@ -11261,7 +11276,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="135">
         <v>2016</v>
       </c>
@@ -11333,7 +11348,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="135">
         <v>2016</v>
       </c>
@@ -11408,7 +11423,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="23" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="135">
         <v>2016</v>
       </c>
@@ -11480,7 +11495,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="135">
         <v>2016</v>
       </c>
@@ -11553,7 +11568,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="135">
         <v>2016</v>
       </c>
@@ -11626,7 +11641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="135">
         <v>2016</v>
       </c>
@@ -11701,7 +11716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="135">
         <v>2016</v>
       </c>
@@ -11773,7 +11788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="135">
         <v>2016</v>
       </c>
@@ -11845,7 +11860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="135">
         <v>2016</v>
       </c>
@@ -11912,7 +11927,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="135">
         <v>2016</v>
       </c>
@@ -11979,7 +11994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="135">
         <v>2016</v>
       </c>
@@ -12051,7 +12066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="135">
         <v>2016</v>
       </c>
@@ -12118,7 +12133,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="135">
         <v>2016</v>
       </c>
@@ -12190,7 +12205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="135">
         <v>2016</v>
       </c>
@@ -12262,7 +12277,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="135">
         <v>2016</v>
       </c>
@@ -12330,7 +12345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="135">
         <v>2016</v>
       </c>
@@ -12398,7 +12413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:28" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:28" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="135">
         <v>2016</v>
       </c>
@@ -12470,7 +12485,7 @@
       <c r="AA37" s="46"/>
       <c r="AB37" s="46"/>
     </row>
-    <row r="38" spans="1:28" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:28" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="135">
         <v>2016</v>
       </c>
@@ -12541,7 +12556,7 @@
       <c r="AA38" s="46"/>
       <c r="AB38" s="46"/>
     </row>
-    <row r="39" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="135">
         <v>2016</v>
       </c>
@@ -12606,7 +12621,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="135">
         <v>2016</v>
       </c>
@@ -12673,7 +12688,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="135">
         <v>2016</v>
       </c>
@@ -12740,7 +12755,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="135">
         <v>2016</v>
       </c>
@@ -12810,7 +12825,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="43" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="135">
         <v>2016</v>
       </c>
@@ -12877,7 +12892,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="135">
         <v>2016</v>
       </c>
@@ -12944,7 +12959,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="45" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="135">
         <v>2016</v>
       </c>
@@ -13016,7 +13031,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="135">
         <v>2016</v>
       </c>
@@ -13083,7 +13098,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="135">
         <v>2016</v>
       </c>
@@ -13151,7 +13166,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="135">
         <v>2016</v>
       </c>
@@ -13219,7 +13234,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="135">
         <v>2016</v>
       </c>
@@ -13289,7 +13304,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="135">
         <v>2016</v>
       </c>
@@ -13356,7 +13371,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="135">
         <v>2016</v>
       </c>
@@ -13428,7 +13443,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="135">
         <v>2016</v>
       </c>
@@ -13497,7 +13512,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="53" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="135">
         <v>2016</v>
       </c>
@@ -13566,7 +13581,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="54" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="135">
         <v>2016</v>
       </c>
@@ -13632,7 +13647,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="55" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="135">
         <v>2016</v>
       </c>
@@ -13706,7 +13721,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="56" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="135">
         <v>2016</v>
       </c>
@@ -13777,7 +13792,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="57" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="135">
         <v>2016</v>
       </c>
@@ -13848,7 +13863,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="58" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="135">
         <v>2016</v>
       </c>
@@ -13920,7 +13935,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="59" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="135">
         <v>2016</v>
       </c>
@@ -13992,7 +14007,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="60" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="135">
         <v>2016</v>
       </c>
@@ -14053,7 +14068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="135">
         <v>2016</v>
       </c>
@@ -14111,7 +14126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="135">
         <v>2016</v>
       </c>
@@ -14169,7 +14184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="135">
         <v>2016</v>
       </c>
@@ -14227,7 +14242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="135">
         <v>2016</v>
       </c>
@@ -14285,7 +14300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="135">
         <v>2016</v>
       </c>
@@ -14343,7 +14358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="135">
         <v>2016</v>
       </c>
@@ -14399,7 +14414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" s="135">
         <v>2016</v>
       </c>
@@ -14457,7 +14472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:28" s="107" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:28" s="107" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="135">
         <v>2016</v>
       </c>
@@ -14519,7 +14534,7 @@
       <c r="AA68" s="116"/>
       <c r="AB68" s="116"/>
     </row>
-    <row r="69" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="135">
         <v>2016</v>
       </c>
@@ -14573,7 +14588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="135">
         <v>2016</v>
       </c>
@@ -14630,7 +14645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="135">
         <v>2016</v>
       </c>
@@ -14689,7 +14704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="135">
         <v>2016</v>
       </c>
@@ -14747,7 +14762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" s="135">
         <v>2016</v>
       </c>
@@ -14805,7 +14820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" s="135">
         <v>2016</v>
       </c>
@@ -14863,7 +14878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" s="135">
         <v>2016</v>
       </c>
@@ -14921,7 +14936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" s="135">
         <v>2016</v>
       </c>
@@ -14979,7 +14994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A77" s="135">
         <v>2016</v>
       </c>
@@ -15037,7 +15052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:28" s="107" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:28" s="107" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" s="135">
         <v>2016</v>
       </c>
@@ -15099,7 +15114,7 @@
       <c r="AA78" s="116"/>
       <c r="AB78" s="116"/>
     </row>
-    <row r="79" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" s="135">
         <v>2016</v>
       </c>
@@ -15158,7 +15173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" s="135">
         <v>2016</v>
       </c>
@@ -15219,7 +15234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A81" s="135">
         <v>2016</v>
       </c>
@@ -15277,7 +15292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" s="135">
         <v>2016</v>
       </c>
@@ -15339,7 +15354,7 @@
       <c r="AA82"/>
       <c r="AB82"/>
     </row>
-    <row r="83" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" s="135">
         <v>2016</v>
       </c>
@@ -15401,7 +15416,7 @@
       <c r="AA83"/>
       <c r="AB83"/>
     </row>
-    <row r="84" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A84" s="135">
         <v>2016</v>
       </c>
@@ -15461,7 +15476,7 @@
       <c r="AA84"/>
       <c r="AB84"/>
     </row>
-    <row r="85" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A85" s="135">
         <v>2016</v>
       </c>
@@ -15524,7 +15539,7 @@
       <c r="AA85"/>
       <c r="AB85"/>
     </row>
-    <row r="86" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A86" s="135">
         <v>2016</v>
       </c>
@@ -15568,7 +15583,7 @@
       <c r="AA86"/>
       <c r="AB86"/>
     </row>
-    <row r="87" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A87" s="135">
         <v>2016</v>
       </c>
@@ -15612,7 +15627,7 @@
       <c r="AA87"/>
       <c r="AB87"/>
     </row>
-    <row r="88" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A88" s="135">
         <v>2016</v>
       </c>
@@ -15656,7 +15671,7 @@
       <c r="AA88"/>
       <c r="AB88"/>
     </row>
-    <row r="89" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A89" s="135">
         <v>2016</v>
       </c>
@@ -15696,7 +15711,7 @@
       <c r="W89"/>
       <c r="X89"/>
     </row>
-    <row r="90" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A90" s="135">
         <v>2016</v>
       </c>
@@ -15734,7 +15749,7 @@
       <c r="W90"/>
       <c r="X90"/>
     </row>
-    <row r="91" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A91" s="135">
         <v>2016</v>
       </c>
@@ -15772,7 +15787,7 @@
       <c r="W91"/>
       <c r="X91"/>
     </row>
-    <row r="92" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A92" s="135">
         <v>2016</v>
       </c>
@@ -15809,7 +15824,7 @@
       <c r="V92" s="9"/>
       <c r="W92" s="9"/>
     </row>
-    <row r="93" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A93" s="135">
         <v>2016</v>
       </c>
@@ -15846,7 +15861,7 @@
       <c r="V93" s="9"/>
       <c r="W93" s="9"/>
     </row>
-    <row r="94" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A94" s="135">
         <v>2016</v>
       </c>
@@ -15885,7 +15900,7 @@
       <c r="V94" s="9"/>
       <c r="W94" s="9"/>
     </row>
-    <row r="95" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A95" s="135">
         <v>2016</v>
       </c>
@@ -15924,7 +15939,7 @@
       <c r="V95" s="9"/>
       <c r="W95" s="9"/>
     </row>
-    <row r="96" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A96" s="135">
         <v>2016</v>
       </c>
@@ -15963,7 +15978,7 @@
       <c r="V96" s="9"/>
       <c r="W96" s="9"/>
     </row>
-    <row r="97" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A97" s="135">
         <v>2016</v>
       </c>
@@ -16002,7 +16017,7 @@
       <c r="V97" s="9"/>
       <c r="W97" s="9"/>
     </row>
-    <row r="98" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A98" s="135">
         <v>2016</v>
       </c>
@@ -16041,7 +16056,7 @@
       <c r="V98" s="9"/>
       <c r="W98" s="9"/>
     </row>
-    <row r="99" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A99" s="135">
         <v>2016</v>
       </c>
@@ -16080,7 +16095,7 @@
       <c r="V99" s="9"/>
       <c r="W99" s="9"/>
     </row>
-    <row r="100" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A100" s="135">
         <v>2016</v>
       </c>
@@ -16119,7 +16134,7 @@
       <c r="V100" s="9"/>
       <c r="W100" s="9"/>
     </row>
-    <row r="101" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A101" s="135">
         <v>2016</v>
       </c>
@@ -16158,7 +16173,7 @@
       <c r="V101" s="9"/>
       <c r="W101" s="9"/>
     </row>
-    <row r="102" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A102" s="135">
         <v>2016</v>
       </c>
@@ -16195,7 +16210,7 @@
       <c r="V102" s="9"/>
       <c r="W102" s="9"/>
     </row>
-    <row r="103" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A103" s="135">
         <v>2016</v>
       </c>
@@ -16234,7 +16249,7 @@
       <c r="V103" s="9"/>
       <c r="W103" s="9"/>
     </row>
-    <row r="104" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A104" s="135">
         <v>2016</v>
       </c>
@@ -16273,7 +16288,7 @@
       <c r="V104" s="9"/>
       <c r="W104" s="9"/>
     </row>
-    <row r="105" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A105" s="135">
         <v>2016</v>
       </c>
@@ -16312,7 +16327,7 @@
       <c r="V105" s="9"/>
       <c r="W105" s="9"/>
     </row>
-    <row r="106" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A106" s="135">
         <v>2016</v>
       </c>
@@ -16349,7 +16364,7 @@
       <c r="V106" s="9"/>
       <c r="W106" s="9"/>
     </row>
-    <row r="107" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A107" s="135">
         <v>2016</v>
       </c>
@@ -16386,7 +16401,7 @@
       <c r="V107" s="9"/>
       <c r="W107" s="9"/>
     </row>
-    <row r="108" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A108" s="135">
         <v>2016</v>
       </c>
@@ -16420,7 +16435,7 @@
       <c r="V108" s="9"/>
       <c r="W108" s="9"/>
     </row>
-    <row r="109" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A109" s="135">
         <v>2016</v>
       </c>
@@ -16454,7 +16469,7 @@
       <c r="V109" s="9"/>
       <c r="W109" s="9"/>
     </row>
-    <row r="110" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A110" s="135">
         <v>2016</v>
       </c>
@@ -16489,7 +16504,7 @@
       <c r="V110" s="9"/>
       <c r="W110" s="9"/>
     </row>
-    <row r="111" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A111" s="135">
         <v>2016</v>
       </c>
@@ -16524,7 +16539,7 @@
       <c r="V111" s="9"/>
       <c r="W111" s="9"/>
     </row>
-    <row r="112" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A112" s="135">
         <v>2016</v>
       </c>
@@ -16558,7 +16573,7 @@
       <c r="V112" s="9"/>
       <c r="W112" s="9"/>
     </row>
-    <row r="113" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A113" s="135">
         <v>2016</v>
       </c>
@@ -16592,7 +16607,7 @@
       <c r="V113" s="9"/>
       <c r="W113" s="9"/>
     </row>
-    <row r="114" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A114" s="135">
         <v>2016</v>
       </c>
@@ -16626,7 +16641,7 @@
       <c r="V114" s="9"/>
       <c r="W114" s="9"/>
     </row>
-    <row r="115" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M115" s="9"/>
       <c r="N115" s="28"/>
       <c r="O115" s="28"/>
@@ -16639,7 +16654,7 @@
       <c r="V115" s="9"/>
       <c r="W115" s="9"/>
     </row>
-    <row r="116" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M116" s="9"/>
       <c r="N116" s="28"/>
       <c r="O116" s="28"/>
@@ -16652,7 +16667,7 @@
       <c r="V116" s="9"/>
       <c r="W116" s="9"/>
     </row>
-    <row r="117" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M117" s="9"/>
       <c r="N117" s="28"/>
       <c r="O117" s="28"/>
@@ -16665,7 +16680,7 @@
       <c r="V117" s="9"/>
       <c r="W117" s="9"/>
     </row>
-    <row r="118" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M118" s="9"/>
       <c r="N118" s="28"/>
       <c r="O118" s="28"/>
@@ -16678,7 +16693,7 @@
       <c r="V118" s="9"/>
       <c r="W118" s="9"/>
     </row>
-    <row r="119" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M119" s="9"/>
       <c r="N119" s="28"/>
       <c r="O119" s="28"/>
@@ -16691,7 +16706,7 @@
       <c r="V119" s="9"/>
       <c r="W119" s="9"/>
     </row>
-    <row r="120" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M120" s="9"/>
       <c r="N120" s="28"/>
       <c r="O120" s="28"/>
@@ -16704,7 +16719,7 @@
       <c r="V120" s="9"/>
       <c r="W120" s="9"/>
     </row>
-    <row r="121" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M121" s="9"/>
       <c r="N121" s="28"/>
       <c r="O121" s="28"/>
@@ -16717,7 +16732,7 @@
       <c r="V121" s="9"/>
       <c r="W121" s="9"/>
     </row>
-    <row r="122" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M122" s="9"/>
       <c r="N122" s="28"/>
       <c r="O122" s="28"/>
@@ -16730,7 +16745,7 @@
       <c r="V122" s="9"/>
       <c r="W122" s="9"/>
     </row>
-    <row r="123" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M123" s="9"/>
       <c r="N123" s="28"/>
       <c r="O123" s="28"/>
@@ -16743,7 +16758,7 @@
       <c r="V123" s="9"/>
       <c r="W123" s="9"/>
     </row>
-    <row r="124" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M124" s="9"/>
       <c r="N124" s="28"/>
       <c r="O124" s="28"/>
@@ -16756,7 +16771,7 @@
       <c r="V124" s="9"/>
       <c r="W124" s="9"/>
     </row>
-    <row r="125" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M125" s="9"/>
       <c r="N125" s="28"/>
       <c r="O125" s="28"/>
@@ -16769,7 +16784,7 @@
       <c r="V125" s="9"/>
       <c r="W125" s="9"/>
     </row>
-    <row r="126" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M126" s="9"/>
       <c r="N126" s="28"/>
       <c r="O126" s="28"/>
@@ -16782,7 +16797,7 @@
       <c r="V126" s="9"/>
       <c r="W126" s="9"/>
     </row>
-    <row r="127" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M127" s="9"/>
       <c r="N127" s="28"/>
       <c r="O127" s="28"/>
@@ -16795,7 +16810,7 @@
       <c r="V127" s="9"/>
       <c r="W127" s="9"/>
     </row>
-    <row r="128" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M128" s="9"/>
       <c r="N128" s="28"/>
       <c r="O128" s="28"/>
@@ -16808,7 +16823,7 @@
       <c r="V128" s="9"/>
       <c r="W128" s="9"/>
     </row>
-    <row r="129" spans="13:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="13:23" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M129" s="9"/>
       <c r="N129" s="28"/>
       <c r="O129" s="28"/>
@@ -16821,7 +16836,7 @@
       <c r="V129" s="9"/>
       <c r="W129" s="9"/>
     </row>
-    <row r="130" spans="13:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="13:23" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M130" s="9"/>
       <c r="N130" s="28"/>
       <c r="O130" s="28"/>
@@ -16834,7 +16849,7 @@
       <c r="V130" s="9"/>
       <c r="W130" s="9"/>
     </row>
-    <row r="131" spans="13:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="13:23" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M131" s="9"/>
       <c r="N131" s="28"/>
       <c r="O131" s="28"/>
@@ -16847,7 +16862,7 @@
       <c r="V131" s="9"/>
       <c r="W131" s="9"/>
     </row>
-    <row r="132" spans="13:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="13:23" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M132" s="9"/>
       <c r="N132" s="28"/>
       <c r="O132" s="28"/>
@@ -16860,7 +16875,7 @@
       <c r="V132" s="9"/>
       <c r="W132" s="9"/>
     </row>
-    <row r="133" spans="13:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="13:23" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M133" s="9"/>
       <c r="N133" s="28"/>
       <c r="O133" s="28"/>
@@ -16873,7 +16888,7 @@
       <c r="V133" s="9"/>
       <c r="W133" s="9"/>
     </row>
-    <row r="134" spans="13:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="13:23" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M134" s="9"/>
       <c r="N134" s="28"/>
       <c r="O134" s="28"/>
@@ -16886,7 +16901,7 @@
       <c r="V134" s="9"/>
       <c r="W134" s="9"/>
     </row>
-    <row r="135" spans="13:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="13:23" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M135" s="9"/>
       <c r="N135" s="28"/>
       <c r="O135" s="28"/>
@@ -16899,7 +16914,7 @@
       <c r="V135" s="9"/>
       <c r="W135" s="9"/>
     </row>
-    <row r="136" spans="13:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="13:23" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M136" s="9"/>
       <c r="N136" s="28"/>
       <c r="O136" s="28"/>
@@ -16912,7 +16927,7 @@
       <c r="V136" s="9"/>
       <c r="W136" s="9"/>
     </row>
-    <row r="137" spans="13:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="13:23" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M137" s="9"/>
       <c r="N137" s="28"/>
       <c r="O137" s="28"/>
@@ -16925,7 +16940,7 @@
       <c r="V137" s="9"/>
       <c r="W137" s="9"/>
     </row>
-    <row r="138" spans="13:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="13:23" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M138" s="9"/>
       <c r="N138" s="28"/>
       <c r="O138" s="28"/>
@@ -16938,7 +16953,7 @@
       <c r="V138" s="9"/>
       <c r="W138" s="9"/>
     </row>
-    <row r="139" spans="13:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="13:23" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M139" s="9"/>
       <c r="N139" s="28"/>
       <c r="O139" s="28"/>
@@ -16951,7 +16966,7 @@
       <c r="V139" s="9"/>
       <c r="W139" s="9"/>
     </row>
-    <row r="140" spans="13:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="13:23" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M140" s="9"/>
       <c r="N140" s="28"/>
       <c r="O140" s="28"/>
@@ -16964,7 +16979,7 @@
       <c r="V140" s="9"/>
       <c r="W140" s="9"/>
     </row>
-    <row r="141" spans="13:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="13:23" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M141" s="9"/>
       <c r="N141" s="28"/>
       <c r="O141" s="28"/>
@@ -16977,14 +16992,14 @@
       <c r="V141" s="9"/>
       <c r="W141" s="9"/>
     </row>
-    <row r="192" spans="11:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="192" spans="11:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="K192" s="17"/>
       <c r="Y192"/>
       <c r="Z192"/>
       <c r="AA192"/>
       <c r="AB192"/>
     </row>
-    <row r="195" spans="12:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="195" spans="12:24" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="L195" s="16"/>
       <c r="N195" s="16"/>
       <c r="O195" s="16"/>
@@ -16999,7 +17014,7 @@
       <c r="X195"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:H113"/>
+  <autoFilter ref="A2:H113" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <mergeCells count="3">
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="R1:U1"/>
@@ -17011,19 +17026,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="Q34" sqref="Q34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="12" max="13" width="8.83203125" style="10"/>
+    <col min="12" max="13" width="8.81640625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>39</v>
       </c>
@@ -17032,7 +17047,7 @@
       <c r="L1" s="10"/>
       <c r="M1" s="10"/>
     </row>
-    <row r="2" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>40</v>
       </c>
@@ -17045,7 +17060,7 @@
       <c r="L2" s="10"/>
       <c r="M2" s="10"/>
     </row>
-    <row r="3" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>43</v>
       </c>
@@ -17054,7 +17069,7 @@
       <c r="L3" s="10"/>
       <c r="M3" s="10"/>
     </row>
-    <row r="4" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>29</v>
       </c>
@@ -17074,7 +17089,7 @@
       <c r="L4" s="10"/>
       <c r="M4" s="10"/>
     </row>
-    <row r="5" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>22</v>
       </c>
@@ -17094,7 +17109,7 @@
       <c r="L5" s="10"/>
       <c r="M5" s="10"/>
     </row>
-    <row r="6" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>28</v>
       </c>
@@ -17114,7 +17129,7 @@
       <c r="L6" s="10"/>
       <c r="M6" s="10"/>
     </row>
-    <row r="7" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>23</v>
       </c>
@@ -17134,7 +17149,7 @@
       <c r="L7" s="10"/>
       <c r="M7" s="10"/>
     </row>
-    <row r="8" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>30</v>
       </c>
@@ -17154,7 +17169,7 @@
       <c r="L8" s="10"/>
       <c r="M8" s="10"/>
     </row>
-    <row r="9" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>24</v>
       </c>
@@ -17174,7 +17189,7 @@
       <c r="L9" s="10"/>
       <c r="M9" s="10"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>25</v>
       </c>
@@ -17192,7 +17207,7 @@
         <v>29.35</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>27</v>
       </c>
@@ -17210,7 +17225,7 @@
         <v>26.650000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>31</v>
       </c>
@@ -17228,7 +17243,7 @@
         <v>36.450000000000003</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>26</v>
       </c>
@@ -17239,7 +17254,7 @@
         <v>10.1</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>241</v>
       </c>
@@ -17250,7 +17265,7 @@
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
     </row>
-    <row r="17" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3"/>
       <c r="B17" s="192">
         <v>2013</v>
@@ -17275,7 +17290,7 @@
       <c r="N17" s="43"/>
       <c r="O17" s="43"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>40</v>
       </c>
@@ -17308,7 +17323,7 @@
       <c r="N18" s="10"/>
       <c r="O18" s="10"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A19" s="47" t="s">
         <v>29</v>
       </c>
@@ -17348,7 +17363,7 @@
       <c r="N19" s="10"/>
       <c r="O19" s="10"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A20" s="47" t="s">
         <v>28</v>
       </c>
@@ -17388,7 +17403,7 @@
       <c r="N20" s="10"/>
       <c r="O20" s="10"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A21" s="47" t="s">
         <v>30</v>
       </c>
@@ -17428,7 +17443,7 @@
       <c r="N21" s="10"/>
       <c r="O21" s="10"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A22" s="47" t="s">
         <v>26</v>
       </c>
@@ -17468,7 +17483,7 @@
       <c r="N22" s="10"/>
       <c r="O22" s="10"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23" s="109" t="s">
         <v>31</v>
       </c>
@@ -17508,7 +17523,7 @@
       <c r="N23" s="10"/>
       <c r="O23" s="10"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A24" s="59" t="s">
         <v>23</v>
       </c>
@@ -17544,7 +17559,7 @@
       <c r="N24" s="10"/>
       <c r="O24" s="10"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A25" s="59" t="s">
         <v>24</v>
       </c>
@@ -17580,7 +17595,7 @@
       <c r="N25" s="10"/>
       <c r="O25" s="10"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A26" s="59" t="s">
         <v>25</v>
       </c>
@@ -17616,7 +17631,7 @@
       <c r="N26" s="10"/>
       <c r="O26" s="10"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A27" s="59" t="s">
         <v>27</v>
       </c>
@@ -17652,7 +17667,7 @@
       <c r="N27" s="10"/>
       <c r="O27" s="10"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A28" s="59" t="s">
         <v>112</v>
       </c>
@@ -17684,7 +17699,7 @@
       <c r="N28" s="10"/>
       <c r="O28" s="10"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A29" s="62" t="s">
         <v>43</v>
       </c>
@@ -17716,7 +17731,7 @@
       <c r="N29" s="10"/>
       <c r="O29" s="10"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A30" s="59" t="s">
         <v>22</v>
       </c>
@@ -17752,7 +17767,7 @@
       <c r="N30" s="10"/>
       <c r="O30" s="10"/>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A31" s="109"/>
       <c r="B31" s="124"/>
       <c r="C31" s="124"/>
@@ -17770,7 +17785,7 @@
         <v>30.650000000000002</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A32" s="58"/>
       <c r="B32" t="s">
         <v>240</v>
@@ -17783,28 +17798,28 @@
         <v>42.45</v>
       </c>
     </row>
-    <row r="33" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="12:13" x14ac:dyDescent="0.35">
       <c r="L33"/>
       <c r="M33" s="80"/>
     </row>
-    <row r="34" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="12:13" x14ac:dyDescent="0.35">
       <c r="L34"/>
       <c r="M34" s="80"/>
     </row>
-    <row r="35" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="12:13" x14ac:dyDescent="0.35">
       <c r="L35"/>
       <c r="M35" s="80"/>
     </row>
-    <row r="36" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="12:13" x14ac:dyDescent="0.35">
       <c r="L36"/>
       <c r="M36" s="80"/>
     </row>
-    <row r="37" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="37" spans="12:13" x14ac:dyDescent="0.35">
       <c r="L37"/>
       <c r="M37" s="80"/>
     </row>
   </sheetData>
-  <sortState ref="A3:C12">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:C12">
     <sortCondition ref="A3"/>
   </sortState>
   <mergeCells count="4">
@@ -17820,26 +17835,26 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" style="10" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.1640625" style="10"/>
-    <col min="5" max="5" width="9.83203125" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.1640625" style="154"/>
-    <col min="7" max="7" width="13.83203125" style="10" customWidth="1"/>
-    <col min="8" max="10" width="14.6640625" style="10" customWidth="1"/>
-    <col min="11" max="16384" width="9.1640625" style="10"/>
+    <col min="1" max="1" width="13.36328125" style="10" customWidth="1"/>
+    <col min="2" max="2" width="14.81640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.1796875" style="10"/>
+    <col min="5" max="5" width="9.81640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1796875" style="154"/>
+    <col min="7" max="7" width="13.81640625" style="10" customWidth="1"/>
+    <col min="8" max="10" width="14.6328125" style="10" customWidth="1"/>
+    <col min="11" max="16384" width="9.1796875" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -17871,7 +17886,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
         <v>18</v>
       </c>
@@ -17903,7 +17918,7 @@
         <v>-120.321929999999</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
         <v>18</v>
       </c>
@@ -17935,7 +17950,7 @@
         <v>-120.37219</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
         <v>18</v>
       </c>
@@ -17967,7 +17982,7 @@
         <v>-120.456999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
         <v>18</v>
       </c>
@@ -17999,7 +18014,7 @@
         <v>-120.57396</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
         <v>18</v>
       </c>
@@ -18031,7 +18046,7 @@
         <v>-120.60517</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="91" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" s="91" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="91" t="s">
         <v>18</v>
       </c>
@@ -18063,7 +18078,7 @@
         <v>-120.6502</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
         <v>18</v>
       </c>
@@ -18095,7 +18110,7 @@
         <v>-120.65965</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="10" t="s">
         <v>18</v>
       </c>
@@ -18127,7 +18142,7 @@
         <v>-120.67433</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="101" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" s="101" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="101" t="s">
         <v>18</v>
       </c>
@@ -18159,7 +18174,7 @@
         <v>-120.723299999999</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="101" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" s="101" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="101" t="s">
         <v>18</v>
       </c>
@@ -18191,7 +18206,7 @@
         <v>-120.72451</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="10" t="s">
         <v>18</v>
       </c>
@@ -18223,7 +18238,7 @@
         <v>-120.73014000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="10" t="s">
         <v>18</v>
       </c>
@@ -18255,7 +18270,7 @@
         <v>-120.73445</v>
       </c>
     </row>
-    <row r="14" spans="1:10" s="91" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" s="91" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="91" t="s">
         <v>18</v>
       </c>
@@ -18287,7 +18302,7 @@
         <v>-120.66564</v>
       </c>
     </row>
-    <row r="15" spans="1:10" s="91" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" s="91" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="91" t="s">
         <v>18</v>
       </c>
@@ -18319,7 +18334,7 @@
         <v>-120.65971</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="83" t="s">
         <v>18</v>
       </c>
@@ -18351,7 +18366,7 @@
         <v>-120.65006</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="10" t="s">
         <v>73</v>
       </c>
@@ -18371,7 +18386,7 @@
         <v>-119.9224</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="10" t="s">
         <v>73</v>
       </c>
@@ -18391,7 +18406,7 @@
         <v>-120.0209</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="10" t="s">
         <v>73</v>
       </c>
@@ -18411,7 +18426,7 @@
         <v>-120.01609999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="10" t="s">
         <v>73</v>
       </c>
@@ -18431,7 +18446,7 @@
         <v>-120.12520000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" s="10" t="s">
         <v>73</v>
       </c>
@@ -18451,7 +18466,7 @@
         <v>-120.1173</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="10" t="s">
         <v>73</v>
       </c>
@@ -18471,7 +18486,7 @@
         <v>-120.0664</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" s="10" t="s">
         <v>73</v>
       </c>
@@ -18491,7 +18506,7 @@
         <v>-120.1066</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" s="10" t="s">
         <v>73</v>
       </c>
@@ -18511,7 +18526,7 @@
         <v>-120.18810000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" s="10" t="s">
         <v>82</v>
       </c>

</xml_diff>